<commit_message>
update commander and sequential
</commit_message>
<xml_diff>
--- a/out/results.xlsx
+++ b/out/results.xlsx
@@ -412,10 +412,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="A2:F10"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -459,7 +459,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>7-4-2</t>
+          <t>5-4-4</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -469,25 +469,25 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.109</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>unsat</t>
+          <t>sat</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>560</v>
+        <v>1600</v>
       </c>
       <c r="F2" t="n">
-        <v>7412</v>
+        <v>35192</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>7-4-2</t>
+          <t>4-3-3</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -497,25 +497,25 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.002</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>unsat</t>
+          <t>sat</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>560</v>
+        <v>432</v>
       </c>
       <c r="F3" t="n">
-        <v>14824</v>
+        <v>6219</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>7-4-2</t>
+          <t>7-2-4</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -525,25 +525,25 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.001</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>unsat</t>
+          <t>sat</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>560</v>
+        <v>672</v>
       </c>
       <c r="F4" t="n">
-        <v>7412</v>
+        <v>14916</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>15-8-2</t>
+          <t>9-2-5</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -553,25 +553,25 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.011</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>unsat</t>
+          <t>sat</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>4320</v>
+        <v>1350</v>
       </c>
       <c r="F5" t="n">
-        <v>131624</v>
+        <v>54215</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>5-3-6</t>
+          <t>5-4-5</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -581,7 +581,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.047</t>
+          <t>0.641</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -590,16 +590,16 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>2160</v>
+        <v>2500</v>
       </c>
       <c r="F6" t="n">
-        <v>98109</v>
+        <v>74054</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>7-4-2</t>
+          <t>1-3-5</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -618,16 +618,16 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>-1</v>
+        <v>300</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>4875</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>15-8-2</t>
+          <t>2-3-5</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -646,16 +646,16 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>-1</v>
+        <v>600</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>12495</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>5-3-6</t>
+          <t>3-3-5</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>-1</v>
+        <v>900</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>22740</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>7-4-2</t>
+          <t>4-3-5</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -693,25 +693,25 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.001</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>unsat</t>
+          <t>sat</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>560</v>
+        <v>1200</v>
       </c>
       <c r="F10" t="n">
-        <v>7412</v>
+        <v>35610</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>15-8-2</t>
+          <t>5-3-5</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -721,25 +721,25 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.024</t>
+          <t>0.031</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>unsat</t>
+          <t>sat</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>4320</v>
+        <v>1500</v>
       </c>
       <c r="F11" t="n">
-        <v>131624</v>
+        <v>51105</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>5-3-6</t>
+          <t>6-3-5</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -749,7 +749,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.062</t>
+          <t>0.250</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -758,16 +758,16 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>2160</v>
+        <v>1800</v>
       </c>
       <c r="F12" t="n">
-        <v>98109</v>
+        <v>42248</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>7-4-2</t>
+          <t>6-4-8</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -777,19 +777,19 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.001</t>
+          <t>6.234</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>unsat</t>
+          <t>sat</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>560</v>
+        <v>7680</v>
       </c>
       <c r="F13" t="n">
-        <v>7412</v>
+        <v>593261</v>
       </c>
     </row>
     <row r="14">
@@ -823,7 +823,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>7-4-2</t>
+          <t>15-8-2</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -833,7 +833,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>0.002</t>
+          <t>0.016</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -842,16 +842,16 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>560</v>
+        <v>4320</v>
       </c>
       <c r="F15" t="n">
-        <v>7412</v>
+        <v>131624</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>7-4-2</t>
+          <t>5-3-6</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -861,63 +861,63 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>0.003</t>
+          <t>0.062</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>unsat</t>
+          <t>sat</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>560</v>
+        <v>2160</v>
       </c>
       <c r="F16" t="n">
-        <v>7412</v>
+        <v>98109</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>15-8-2</t>
+          <t>5-4-4</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>binary</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>0.032</t>
+          <t>0.109</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>unsat</t>
+          <t>sat</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>4320</v>
+        <v>1600</v>
       </c>
       <c r="F17" t="n">
-        <v>131624</v>
+        <v>35192</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>5-3-6</t>
+          <t>4-3-3</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>binary</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>0.047</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -926,82 +926,82 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>2160</v>
+        <v>432</v>
       </c>
       <c r="F18" t="n">
-        <v>98109</v>
+        <v>6219</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>7-4-2</t>
+          <t>7-2-4</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>binary</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>0.001</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>unsat</t>
+          <t>sat</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>560</v>
+        <v>672</v>
       </c>
       <c r="F19" t="n">
-        <v>7412</v>
+        <v>14916</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>15-8-2</t>
+          <t>9-2-5</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>binary</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0.014</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>unsat</t>
+          <t>sat</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>4320</v>
+        <v>1350</v>
       </c>
       <c r="F20" t="n">
-        <v>131624</v>
+        <v>54215</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>5-3-6</t>
+          <t>5-4-5</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>binary</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>0.047</t>
+          <t>0.594</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1010,82 +1010,82 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>2160</v>
+        <v>2500</v>
       </c>
       <c r="F21" t="n">
-        <v>98109</v>
+        <v>74054</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>7-4-2</t>
+          <t>1-3-5</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>binary</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0.001</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>unsat</t>
+          <t>sat</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>560</v>
+        <v>300</v>
       </c>
       <c r="F22" t="n">
-        <v>7412</v>
+        <v>4875</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>15-8-2</t>
+          <t>2-3-5</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>binary</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>0.012</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>unsat</t>
+          <t>sat</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>4320</v>
+        <v>600</v>
       </c>
       <c r="F23" t="n">
-        <v>131624</v>
+        <v>12495</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>5-3-6</t>
+          <t>3-3-5</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>binary</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>0.031</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1094,82 +1094,82 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>2160</v>
+        <v>900</v>
       </c>
       <c r="F24" t="n">
-        <v>98109</v>
+        <v>22740</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>7-4-2</t>
+          <t>4-3-5</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>binary</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>0.002</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>unsat</t>
+          <t>sat</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>560</v>
+        <v>1200</v>
       </c>
       <c r="F25" t="n">
-        <v>7412</v>
+        <v>35610</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>15-8-2</t>
+          <t>5-3-5</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>binary</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>0.017</t>
+          <t>0.031</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>unsat</t>
+          <t>sat</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>4320</v>
+        <v>1500</v>
       </c>
       <c r="F26" t="n">
-        <v>131624</v>
+        <v>51105</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5-3-6</t>
+          <t>6-3-5</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>binary</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>0.047</t>
+          <t>0.219</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1178,54 +1178,54 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>2160</v>
+        <v>1800</v>
       </c>
       <c r="F27" t="n">
-        <v>98109</v>
+        <v>42248</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>7-4-2</t>
+          <t>6-4-8</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>binary</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>0.002</t>
+          <t>6.297</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>unsat</t>
+          <t>sat</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>560</v>
+        <v>7680</v>
       </c>
       <c r="F28" t="n">
-        <v>7412</v>
+        <v>593261</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>15-8-2</t>
+          <t>7-4-2</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>binary</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>0.012</t>
+          <t>0.001</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1234,54 +1234,54 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>4320</v>
+        <v>560</v>
       </c>
       <c r="F29" t="n">
-        <v>131624</v>
+        <v>7412</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5-3-6</t>
+          <t>15-8-2</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>binary</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>0.062</t>
+          <t>0.020</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>sat</t>
+          <t>unsat</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>2160</v>
+        <v>4320</v>
       </c>
       <c r="F30" t="n">
-        <v>98109</v>
+        <v>131624</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>5-4-4</t>
+          <t>5-3-6</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>binary</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>0.125</t>
+          <t>0.062</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1290,26 +1290,26 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>1600</v>
+        <v>2160</v>
       </c>
       <c r="F31" t="n">
-        <v>35192</v>
+        <v>98109</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>4-3-3</t>
+          <t>5-4-4</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>commander</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.172</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1318,26 +1318,26 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>432</v>
+        <v>1653</v>
       </c>
       <c r="F32" t="n">
-        <v>6219</v>
+        <v>38602</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>7-2-4</t>
+          <t>4-3-3</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>commander</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.016</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1346,26 +1346,26 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>672</v>
+        <v>942</v>
       </c>
       <c r="F33" t="n">
-        <v>14916</v>
+        <v>6231</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>9-2-5</t>
+          <t>7-2-4</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>commander</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>0.016</t>
+          <t>0.047</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1374,77 +1374,77 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>1350</v>
+        <v>873</v>
       </c>
       <c r="F34" t="n">
-        <v>54215</v>
+        <v>6473</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>5-4-5</t>
+          <t>9-2-5</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>commander</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>0.609</t>
+          <t>10.004</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>sat</t>
+          <t>unsat</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>2500</v>
+        <v>1350</v>
       </c>
       <c r="F35" t="n">
-        <v>74054</v>
+        <v>29733</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1-3-5</t>
+          <t>5-4-5</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>commander</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>10.010</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>sat</t>
+          <t>unsat</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>300</v>
+        <v>2500</v>
       </c>
       <c r="F36" t="n">
-        <v>4875</v>
+        <v>74216</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2-3-5</t>
+          <t>1-3-5</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>commander</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1458,21 +1458,21 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>600</v>
+        <v>1514</v>
       </c>
       <c r="F37" t="n">
-        <v>12495</v>
+        <v>4915</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>3-3-5</t>
+          <t>2-3-5</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>commander</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1486,21 +1486,21 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>900</v>
+        <v>1524</v>
       </c>
       <c r="F38" t="n">
-        <v>22740</v>
+        <v>12535</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>4-3-5</t>
+          <t>3-3-5</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>commander</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1514,26 +1514,26 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>1200</v>
+        <v>1534</v>
       </c>
       <c r="F39" t="n">
-        <v>35610</v>
+        <v>22780</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>5-3-5</t>
+          <t>4-3-5</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>commander</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>0.047</t>
+          <t>0.062</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1542,26 +1542,26 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>1500</v>
+        <v>1544</v>
       </c>
       <c r="F40" t="n">
-        <v>51105</v>
+        <v>31041</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6-3-5</t>
+          <t>5-3-5</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>commander</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>0.219</t>
+          <t>0.078</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1570,26 +1570,26 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>1800</v>
+        <v>1554</v>
       </c>
       <c r="F41" t="n">
-        <v>42248</v>
+        <v>44369</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6-4-8</t>
+          <t>6-3-5</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>commander</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>7.031</t>
+          <t>2.969</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1598,26 +1598,26 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>7680</v>
+        <v>1800</v>
       </c>
       <c r="F42" t="n">
-        <v>593261</v>
+        <v>56047</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>7-4-2</t>
+          <t>6-4-8</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>commander</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>0.002</t>
+          <t>10.005</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1626,26 +1626,26 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>560</v>
+        <v>7680</v>
       </c>
       <c r="F43" t="n">
-        <v>7412</v>
+        <v>675003</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>15-8-2</t>
+          <t>7-4-2</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>commander</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>0.013</t>
+          <t>0.001</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1654,54 +1654,54 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>4320</v>
+        <v>871</v>
       </c>
       <c r="F44" t="n">
-        <v>131624</v>
+        <v>7416</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>5-3-6</t>
+          <t>15-8-2</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>commander</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>0.062</t>
+          <t>0.016</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>sat</t>
+          <t>unsat</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>2160</v>
+        <v>4320</v>
       </c>
       <c r="F45" t="n">
-        <v>98109</v>
+        <v>131628</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>5-4-4</t>
+          <t>5-3-6</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>commander</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>0.125</t>
+          <t>0.172</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1710,26 +1710,26 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>1600</v>
+        <v>2160</v>
       </c>
       <c r="F46" t="n">
-        <v>35192</v>
+        <v>87876</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>4-3-3</t>
+          <t>5-4-4</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>sequential</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>1.656</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1738,26 +1738,26 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>432</v>
+        <v>1653</v>
       </c>
       <c r="F47" t="n">
-        <v>6219</v>
+        <v>23773</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>7-2-4</t>
+          <t>4-3-3</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>sequential</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.016</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1766,105 +1766,105 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>672</v>
+        <v>942</v>
       </c>
       <c r="F48" t="n">
-        <v>14916</v>
+        <v>4569</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>9-2-5</t>
+          <t>7-2-4</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>sequential</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>0.016</t>
+          <t>0.010</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>sat</t>
+          <t>unsat</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>1350</v>
+        <v>873</v>
       </c>
       <c r="F49" t="n">
-        <v>54215</v>
+        <v>13772</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>5-4-5</t>
+          <t>9-2-5</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>sequential</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>0.594</t>
+          <t>0.007</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>sat</t>
+          <t>unsat</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>2500</v>
+        <v>1350</v>
       </c>
       <c r="F50" t="n">
-        <v>74054</v>
+        <v>50255</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>1-3-5</t>
+          <t>5-4-5</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>sequential</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>10.015</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>sat</t>
+          <t>unsat</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>300</v>
+        <v>2500</v>
       </c>
       <c r="F51" t="n">
-        <v>4875</v>
+        <v>65878</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2-3-5</t>
+          <t>1-3-5</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>sequential</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1878,26 +1878,26 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>600</v>
+        <v>1514</v>
       </c>
       <c r="F52" t="n">
-        <v>12495</v>
+        <v>2985</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>3-3-5</t>
+          <t>2-3-5</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>sequential</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.016</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1906,21 +1906,21 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>900</v>
+        <v>1524</v>
       </c>
       <c r="F53" t="n">
-        <v>22740</v>
+        <v>7832</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>4-3-5</t>
+          <t>3-3-5</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>sequential</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1934,26 +1934,26 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>1200</v>
+        <v>1534</v>
       </c>
       <c r="F54" t="n">
-        <v>35610</v>
+        <v>15145</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>5-3-5</t>
+          <t>4-3-5</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>sequential</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>0.031</t>
+          <t>0.078</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1962,26 +1962,26 @@
         </is>
       </c>
       <c r="E55" t="n">
-        <v>1500</v>
+        <v>1544</v>
       </c>
       <c r="F55" t="n">
-        <v>51105</v>
+        <v>24667</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6-3-5</t>
+          <t>5-3-5</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>sequential</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>0.219</t>
+          <t>0.547</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1990,54 +1990,54 @@
         </is>
       </c>
       <c r="E56" t="n">
-        <v>1800</v>
+        <v>1554</v>
       </c>
       <c r="F56" t="n">
-        <v>42248</v>
+        <v>33440</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6-4-8</t>
+          <t>6-3-5</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>sequential</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>6.672</t>
+          <t>10.023</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>sat</t>
+          <t>unsat</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>7680</v>
+        <v>1800</v>
       </c>
       <c r="F57" t="n">
-        <v>593261</v>
+        <v>45034</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>7-4-2</t>
+          <t>6-4-8</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>sequential</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>0.002</t>
+          <t>10.011</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2046,26 +2046,26 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>560</v>
+        <v>7680</v>
       </c>
       <c r="F58" t="n">
-        <v>7412</v>
+        <v>570349</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>15-8-2</t>
+          <t>7-4-2</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>sequential</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>0.013</t>
+          <t>0.001</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2074,54 +2074,54 @@
         </is>
       </c>
       <c r="E59" t="n">
-        <v>4320</v>
+        <v>871</v>
       </c>
       <c r="F59" t="n">
-        <v>131624</v>
+        <v>6964</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>5-3-6</t>
+          <t>15-8-2</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>sequential</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>0.047</t>
+          <t>0.009</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>sat</t>
+          <t>unsat</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>2160</v>
+        <v>4320</v>
       </c>
       <c r="F60" t="n">
-        <v>98109</v>
+        <v>112242</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>5-4-4</t>
+          <t>5-3-6</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>sequential</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>0.109</t>
+          <t>0.328</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2130,26 +2130,26 @@
         </is>
       </c>
       <c r="E61" t="n">
-        <v>1600</v>
+        <v>2160</v>
       </c>
       <c r="F61" t="n">
-        <v>35192</v>
+        <v>70257</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>4-3-3</t>
+          <t>5-4-4</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>product</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>0.125</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2158,21 +2158,21 @@
         </is>
       </c>
       <c r="E62" t="n">
-        <v>432</v>
+        <v>1600</v>
       </c>
       <c r="F62" t="n">
-        <v>6219</v>
+        <v>30096</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>7-2-4</t>
+          <t>4-3-3</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>product</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2186,21 +2186,21 @@
         </is>
       </c>
       <c r="E63" t="n">
-        <v>672</v>
+        <v>432</v>
       </c>
       <c r="F63" t="n">
-        <v>14916</v>
+        <v>3721</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>9-2-5</t>
+          <t>7-2-4</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>product</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2214,26 +2214,26 @@
         </is>
       </c>
       <c r="E64" t="n">
-        <v>1350</v>
+        <v>672</v>
       </c>
       <c r="F64" t="n">
-        <v>54215</v>
+        <v>13124</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>5-4-5</t>
+          <t>9-2-5</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>product</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>0.562</t>
+          <t>3.781</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2242,26 +2242,26 @@
         </is>
       </c>
       <c r="E65" t="n">
-        <v>2500</v>
+        <v>1350</v>
       </c>
       <c r="F65" t="n">
-        <v>74054</v>
+        <v>16509</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>1-3-5</t>
+          <t>5-4-5</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>product</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>0.000</t>
+          <t>2.156</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2270,21 +2270,21 @@
         </is>
       </c>
       <c r="E66" t="n">
-        <v>300</v>
+        <v>2500</v>
       </c>
       <c r="F66" t="n">
-        <v>4875</v>
+        <v>61595</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2-3-5</t>
+          <t>1-3-5</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>product</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2298,21 +2298,21 @@
         </is>
       </c>
       <c r="E67" t="n">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="F67" t="n">
-        <v>12495</v>
+        <v>3255</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>3-3-5</t>
+          <t>2-3-5</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>product</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2326,26 +2326,26 @@
         </is>
       </c>
       <c r="E68" t="n">
-        <v>900</v>
+        <v>600</v>
       </c>
       <c r="F68" t="n">
-        <v>22740</v>
+        <v>9255</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>4-3-5</t>
+          <t>3-3-5</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>product</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>0.016</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2354,21 +2354,21 @@
         </is>
       </c>
       <c r="E69" t="n">
-        <v>1200</v>
+        <v>900</v>
       </c>
       <c r="F69" t="n">
-        <v>35610</v>
+        <v>17880</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>5-3-5</t>
+          <t>4-3-5</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>product</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2382,26 +2382,26 @@
         </is>
       </c>
       <c r="E70" t="n">
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="F70" t="n">
-        <v>51105</v>
+        <v>20070</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6-3-5</t>
+          <t>5-3-5</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>product</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>0.219</t>
+          <t>0.062</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2410,82 +2410,82 @@
         </is>
       </c>
       <c r="E71" t="n">
-        <v>1800</v>
+        <v>1500</v>
       </c>
       <c r="F71" t="n">
-        <v>42248</v>
+        <v>32079</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6-4-8</t>
+          <t>6-3-5</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>product</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>6.531</t>
+          <t>10.044</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>sat</t>
+          <t>unsat</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>7680</v>
+        <v>1800</v>
       </c>
       <c r="F72" t="n">
-        <v>593261</v>
+        <v>39969</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7-4-2</t>
+          <t>6-4-8</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>product</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>0.001</t>
+          <t>8.562</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>unsat</t>
+          <t>sat</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>560</v>
+        <v>7680</v>
       </c>
       <c r="F73" t="n">
-        <v>7412</v>
+        <v>491380</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>15-8-2</t>
+          <t>7-4-2</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>binomial</t>
+          <t>product</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>0.013</t>
+          <t>0.000</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2494,38 +2494,66 @@
         </is>
       </c>
       <c r="E74" t="n">
-        <v>4320</v>
+        <v>560</v>
       </c>
       <c r="F74" t="n">
-        <v>131624</v>
+        <v>5620</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
+          <t>15-8-2</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>product</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>0.012</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>unsat</t>
+        </is>
+      </c>
+      <c r="E75" t="n">
+        <v>4320</v>
+      </c>
+      <c r="F75" t="n">
+        <v>100904</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
           <t>5-3-6</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>binomial</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>0.047</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>sat</t>
-        </is>
-      </c>
-      <c r="E75" t="n">
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>product</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>0.125</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>sat</t>
+        </is>
+      </c>
+      <c r="E76" t="n">
         <v>2160</v>
       </c>
-      <c r="F75" t="n">
-        <v>98109</v>
+      <c r="F76" t="n">
+        <v>60351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>